<commit_message>
fix: bugs, update: st
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\persist-web-dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1742B4A8-3E55-4863-831C-19168F0DAD2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F10C4A-D8FB-4A10-A661-568AAD3C5846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Information" sheetId="1" r:id="rId1"/>
@@ -31,13 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="35">
-  <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="32">
   <si>
     <t>Project ID</t>
   </si>
@@ -48,9 +42,6 @@
     <t>Project Name</t>
   </si>
   <si>
-    <t>Project_Name_Text_Here</t>
-  </si>
-  <si>
     <t>Client ID</t>
   </si>
   <si>
@@ -66,9 +57,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Stage</t>
   </si>
   <si>
@@ -78,9 +66,6 @@
     <t>Drug Image Link</t>
   </si>
   <si>
-    <t>Image_Name</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -135,14 +120,20 @@
     <t>TEXT</t>
   </si>
   <si>
-    <t>02/20/2000</t>
+    <t>https://www.w3schools.com/w3images/popsicle.jpg</t>
+  </si>
+  <si>
+    <t>02/21/2000</t>
+  </si>
+  <si>
+    <t>Project_Name_Text_Here1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -174,6 +165,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -192,10 +190,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -208,8 +207,10 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -428,13 +429,14 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="66.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -450,116 +452,110 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="5">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{FFC4AFD1-0007-4C12-AA6A-26308AF439FD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -568,11 +564,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -581,566 +575,567 @@
     <col min="3" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10000</v>
       </c>
       <c r="B2" s="2">
         <f t="shared" ref="B2:C2" ca="1" si="0">RANDBETWEEN(0,100)</f>
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="C2" s="2">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="D2:D15" ca="1" si="1">RANDBETWEEN(0,10)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E2" s="3">
         <f t="shared" ref="E2:E15" ca="1" si="2">RANDBETWEEN(20,30)</f>
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F2" s="3">
         <f t="shared" ref="F2:F15" ca="1" si="3">RANDBETWEEN(30,40)</f>
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A15" si="4">A2+1</f>
         <v>10001</v>
       </c>
       <c r="B3" s="2">
         <f t="shared" ref="B3:C3" ca="1" si="5">RANDBETWEEN(0,100)</f>
-        <v>2</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" ca="1" si="5"/>
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D3" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <f t="shared" si="4"/>
         <v>10002</v>
       </c>
       <c r="B4" s="2">
         <f t="shared" ref="B4:C4" ca="1" si="6">RANDBETWEEN(0,100)</f>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2">
         <f t="shared" ca="1" si="6"/>
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <f t="shared" si="4"/>
         <v>10003</v>
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5:C5" ca="1" si="7">RANDBETWEEN(0,100)</f>
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="C5" s="2">
         <f t="shared" ca="1" si="7"/>
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <f t="shared" si="4"/>
         <v>10004</v>
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6:C6" ca="1" si="8">RANDBETWEEN(0,100)</f>
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C6" s="2">
         <f t="shared" ca="1" si="8"/>
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <f t="shared" si="4"/>
         <v>10005</v>
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7:C7" ca="1" si="9">RANDBETWEEN(0,100)</f>
-        <v>93</v>
+        <v>28</v>
       </c>
       <c r="C7" s="2">
         <f t="shared" ca="1" si="9"/>
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <f t="shared" si="4"/>
         <v>10006</v>
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8:C8" ca="1" si="10">RANDBETWEEN(0,100)</f>
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C8" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <f t="shared" si="4"/>
         <v>10007</v>
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9:C9" ca="1" si="11">RANDBETWEEN(0,100)</f>
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C9" s="2">
         <f t="shared" ca="1" si="11"/>
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <f t="shared" si="4"/>
         <v>10008</v>
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10:C10" ca="1" si="12">RANDBETWEEN(0,100)</f>
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="C10" s="2">
         <f t="shared" ca="1" si="12"/>
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <f t="shared" si="4"/>
         <v>10009</v>
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11:C11" ca="1" si="13">RANDBETWEEN(0,100)</f>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2">
         <f t="shared" ca="1" si="13"/>
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E11" s="7">
         <v>36589</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <f t="shared" si="4"/>
         <v>10010</v>
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12:C12" ca="1" si="14">RANDBETWEEN(0,100)</f>
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" ca="1" si="14"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <f t="shared" si="4"/>
         <v>10011</v>
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13:C13" ca="1" si="15">RANDBETWEEN(0,100)</f>
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" ca="1" si="15"/>
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="3"/>
         <v>38</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <f t="shared" si="4"/>
         <v>10012</v>
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14:C14" ca="1" si="16">RANDBETWEEN(0,100)</f>
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" ca="1" si="16"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <f t="shared" si="4"/>
         <v>10013</v>
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15:C15" ca="1" si="17">RANDBETWEEN(0,100)</f>
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" ca="1" si="17"/>
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>